<commit_message>
Changed Barry Duffmann to Barry Huffman
</commit_message>
<xml_diff>
--- a/Simpsons.xlsx
+++ b/Simpsons.xlsx
@@ -275,9 +275,6 @@
     <t>27</t>
   </si>
   <si>
-    <t>'Barry Duffman'</t>
-  </si>
-  <si>
     <t>'Duffman'</t>
   </si>
   <si>
@@ -1098,6 +1095,9 @@
   </si>
   <si>
     <t>DROP TABLE IF EXISTS WEARINGS_QUESTIONS; CREATE TABLE WEARINGS_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>Barry Huffman'</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1700,64 +1700,64 @@
         <v>5</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>310</v>
-      </c>
       <c r="K2" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>322</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>313</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>316</v>
-      </c>
-      <c r="S2" s="22" t="s">
+      <c r="U2" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="V2" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="W2" s="14" t="s">
         <v>324</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>318</v>
-      </c>
-      <c r="V2" s="22" t="s">
-        <v>319</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>325</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>6</v>
@@ -1792,7 +1792,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
@@ -1822,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>10</v>
@@ -1867,10 +1867,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>10</v>
@@ -1897,7 +1897,7 @@
         <v>11</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>10</v>
@@ -1906,7 +1906,7 @@
         <v>10</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y4" s="3" t="str">
         <f t="shared" ref="Y4:Y67" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,",",$D4,",",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,",",$U4,",",$V4,",",$W4,"),")</f>
@@ -1942,10 +1942,10 @@
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>10</v>
@@ -1972,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>10</v>
@@ -1981,7 +1981,7 @@
         <v>10</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2017,10 +2017,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>10</v>
@@ -2047,7 +2047,7 @@
         <v>11</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>10</v>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
@@ -2122,7 +2122,7 @@
         <v>11</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>10</v>
@@ -2167,10 +2167,10 @@
         <v>10</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>10</v>
@@ -2197,7 +2197,7 @@
         <v>11</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>10</v>
@@ -2206,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2242,10 +2242,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>10</v>
@@ -2272,7 +2272,7 @@
         <v>11</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>11</v>
@@ -2317,10 +2317,10 @@
         <v>10</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>10</v>
@@ -2347,7 +2347,7 @@
         <v>10</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>10</v>
@@ -2356,7 +2356,7 @@
         <v>10</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2392,10 +2392,10 @@
         <v>10</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>10</v>
@@ -2422,7 +2422,7 @@
         <v>10</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>10</v>
@@ -2467,10 +2467,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>10</v>
@@ -2497,7 +2497,7 @@
         <v>11</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>11</v>
@@ -2542,10 +2542,10 @@
         <v>10</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>11</v>
@@ -2581,7 +2581,7 @@
         <v>10</v>
       </c>
       <c r="W13" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2620,7 +2620,7 @@
         <v>44</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>10</v>
@@ -2647,7 +2647,7 @@
         <v>10</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>10</v>
@@ -2656,7 +2656,7 @@
         <v>10</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2692,10 +2692,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>10</v>
@@ -2722,7 +2722,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U15" s="2" t="s">
         <v>10</v>
@@ -2731,7 +2731,7 @@
         <v>11</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2767,10 +2767,10 @@
         <v>11</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>10</v>
@@ -2797,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>10</v>
@@ -2806,7 +2806,7 @@
         <v>11</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2842,10 +2842,10 @@
         <v>11</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>10</v>
@@ -2872,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U17" s="2" t="s">
         <v>10</v>
@@ -2881,7 +2881,7 @@
         <v>10</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2896,7 +2896,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>14</v>
@@ -2920,7 +2920,7 @@
         <v>44</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
@@ -2947,7 +2947,7 @@
         <v>10</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>10</v>
@@ -2956,7 +2956,7 @@
         <v>10</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2992,10 +2992,10 @@
         <v>10</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>10</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>10</v>
@@ -3031,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3067,10 +3067,10 @@
         <v>10</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>10</v>
@@ -3097,7 +3097,7 @@
         <v>11</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>10</v>
@@ -3145,7 +3145,7 @@
         <v>59</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>10</v>
@@ -3172,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U21" s="2" t="s">
         <v>10</v>
@@ -3181,7 +3181,7 @@
         <v>10</v>
       </c>
       <c r="W21" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3220,7 +3220,7 @@
         <v>59</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>10</v>
@@ -3247,7 +3247,7 @@
         <v>10</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>10</v>
@@ -3322,7 +3322,7 @@
         <v>10</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>10</v>
@@ -3331,7 +3331,7 @@
         <v>10</v>
       </c>
       <c r="W23" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y23" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3397,7 +3397,7 @@
         <v>10</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U24" s="2" t="s">
         <v>10</v>
@@ -3406,7 +3406,7 @@
         <v>10</v>
       </c>
       <c r="W24" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y24" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3445,7 +3445,7 @@
         <v>59</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>10</v>
@@ -3472,7 +3472,7 @@
         <v>10</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U25" s="2" t="s">
         <v>10</v>
@@ -3481,7 +3481,7 @@
         <v>10</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y25" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3517,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>14</v>
@@ -3622,7 +3622,7 @@
         <v>10</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>10</v>
@@ -3668,10 +3668,10 @@
         <v>10</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>10</v>
@@ -3698,7 +3698,7 @@
         <v>10</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>11</v>
@@ -3718,12 +3718,12 @@
       <c r="A30" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D30" s="1" t="s">
         <v>14</v>
       </c>
@@ -3743,10 +3743,10 @@
         <v>10</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>11</v>
@@ -3773,7 +3773,7 @@
         <v>11</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>10</v>
@@ -3782,20 +3782,20 @@
         <v>10</v>
       </c>
       <c r="W30" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>(27,'Barry Duffman','Duffman',null,null,true,true,true,false,'adult','mascot',true,'yellow','blonde',false,false,true,false,true,'athletic',false,false,'glasses'),</v>
+        <v>(27,Barry Huffman','Duffman',null,null,true,true,true,false,'adult','mascot',true,'yellow','blonde',false,false,true,false,true,'athletic',false,false,'glasses'),</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
@@ -3818,10 +3818,10 @@
         <v>10</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>11</v>
@@ -3848,7 +3848,7 @@
         <v>10</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>10</v>
@@ -3857,7 +3857,7 @@
         <v>10</v>
       </c>
       <c r="W31" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3866,10 +3866,10 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
@@ -3896,7 +3896,7 @@
         <v>44</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>10</v>
@@ -3923,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>10</v>
@@ -3932,7 +3932,7 @@
         <v>11</v>
       </c>
       <c r="W32" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3941,11 +3941,11 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
@@ -3968,10 +3968,10 @@
         <v>11</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>10</v>
@@ -3998,7 +3998,7 @@
         <v>11</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U33" s="2" t="s">
         <v>10</v>
@@ -4016,11 +4016,11 @@
     </row>
     <row r="34" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="C34" s="1" t="s">
         <v>14</v>
       </c>
@@ -4043,10 +4043,10 @@
         <v>10</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>11</v>
@@ -4073,7 +4073,7 @@
         <v>11</v>
       </c>
       <c r="T34" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>10</v>
@@ -4091,10 +4091,10 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>14</v>
@@ -4121,7 +4121,7 @@
         <v>44</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>11</v>
@@ -4166,11 +4166,11 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
@@ -4193,10 +4193,10 @@
         <v>10</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>10</v>
@@ -4223,7 +4223,7 @@
         <v>10</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U36" s="2" t="s">
         <v>11</v>
@@ -4241,10 +4241,10 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>14</v>
@@ -4271,7 +4271,7 @@
         <v>44</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>11</v>
@@ -4298,7 +4298,7 @@
         <v>10</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U37" s="2" t="s">
         <v>10</v>
@@ -4307,7 +4307,7 @@
         <v>10</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y37" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4316,14 +4316,14 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D38" s="1" t="s">
         <v>14</v>
       </c>
@@ -4343,10 +4343,10 @@
         <v>10</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>11</v>
@@ -4373,7 +4373,7 @@
         <v>10</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U38" s="2" t="s">
         <v>10</v>
@@ -4382,7 +4382,7 @@
         <v>11</v>
       </c>
       <c r="W38" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y38" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4391,11 +4391,11 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
@@ -4418,10 +4418,10 @@
         <v>10</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>10</v>
@@ -4448,7 +4448,7 @@
         <v>11</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U39" s="2" t="s">
         <v>10</v>
@@ -4457,7 +4457,7 @@
         <v>10</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y39" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4466,14 +4466,14 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D40" s="1" t="s">
         <v>14</v>
       </c>
@@ -4493,10 +4493,10 @@
         <v>10</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>10</v>
@@ -4523,7 +4523,7 @@
         <v>10</v>
       </c>
       <c r="T40" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U40" s="2" t="s">
         <v>10</v>
@@ -4532,7 +4532,7 @@
         <v>11</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y40" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4541,11 +4541,11 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C41" s="1" t="s">
         <v>14</v>
       </c>
@@ -4568,10 +4568,10 @@
         <v>10</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>11</v>
@@ -4598,7 +4598,7 @@
         <v>11</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U41" s="2" t="s">
         <v>11</v>
@@ -4607,7 +4607,7 @@
         <v>10</v>
       </c>
       <c r="W41" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y41" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4616,11 +4616,11 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
@@ -4643,10 +4643,10 @@
         <v>10</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>10</v>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y42" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4691,11 +4691,11 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>14</v>
       </c>
@@ -4718,10 +4718,10 @@
         <v>10</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>11</v>
@@ -4748,7 +4748,7 @@
         <v>10</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>10</v>
@@ -4757,7 +4757,7 @@
         <v>11</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y43" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4766,11 +4766,11 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>14</v>
       </c>
@@ -4793,10 +4793,10 @@
         <v>10</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>10</v>
@@ -4823,7 +4823,7 @@
         <v>11</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U44" s="2" t="s">
         <v>11</v>
@@ -4841,11 +4841,11 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
@@ -4868,10 +4868,10 @@
         <v>10</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>10</v>
@@ -4898,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U45" s="2" t="s">
         <v>10</v>
@@ -4916,11 +4916,11 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
@@ -4943,10 +4943,10 @@
         <v>10</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>10</v>
@@ -4955,7 +4955,7 @@
         <v>12</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>10</v>
@@ -4973,7 +4973,7 @@
         <v>10</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U46" s="2" t="s">
         <v>10</v>
@@ -4991,11 +4991,11 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C47" s="1" t="s">
         <v>14</v>
       </c>
@@ -5018,10 +5018,10 @@
         <v>10</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>11</v>
@@ -5048,7 +5048,7 @@
         <v>11</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>10</v>
@@ -5066,13 +5066,13 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>14</v>
@@ -5096,7 +5096,7 @@
         <v>44</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>11</v>
@@ -5123,7 +5123,7 @@
         <v>10</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U48" s="2" t="s">
         <v>10</v>
@@ -5141,10 +5141,10 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>14</v>
@@ -5171,7 +5171,7 @@
         <v>44</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>11</v>
@@ -5198,7 +5198,7 @@
         <v>10</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U49" s="2" t="s">
         <v>10</v>
@@ -5207,7 +5207,7 @@
         <v>10</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y49" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5216,11 +5216,11 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C50" s="1" t="s">
         <v>14</v>
       </c>
@@ -5243,10 +5243,10 @@
         <v>10</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>10</v>
@@ -5273,7 +5273,7 @@
         <v>10</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>10</v>
@@ -5291,11 +5291,11 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
@@ -5318,10 +5318,10 @@
         <v>10</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>10</v>
@@ -5348,7 +5348,7 @@
         <v>10</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U51" s="2" t="s">
         <v>11</v>
@@ -5366,11 +5366,11 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C52" s="1" t="s">
         <v>14</v>
       </c>
@@ -5393,10 +5393,10 @@
         <v>10</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>11</v>
@@ -5423,7 +5423,7 @@
         <v>11</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>10</v>
@@ -5441,11 +5441,11 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C53" s="1" t="s">
         <v>14</v>
       </c>
@@ -5468,10 +5468,10 @@
         <v>10</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>10</v>
@@ -5480,7 +5480,7 @@
         <v>12</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>10</v>
@@ -5498,7 +5498,7 @@
         <v>10</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U53" s="2" t="s">
         <v>10</v>
@@ -5507,7 +5507,7 @@
         <v>10</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y53" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5516,11 +5516,11 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C54" s="1" t="s">
         <v>14</v>
       </c>
@@ -5543,10 +5543,10 @@
         <v>10</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>10</v>
@@ -5573,7 +5573,7 @@
         <v>10</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U54" s="2" t="s">
         <v>10</v>
@@ -5582,7 +5582,7 @@
         <v>10</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y54" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5591,14 +5591,14 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="D55" s="1" t="s">
         <v>14</v>
       </c>
@@ -5618,10 +5618,10 @@
         <v>11</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>11</v>
@@ -5648,7 +5648,7 @@
         <v>10</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U55" s="2" t="s">
         <v>10</v>
@@ -5666,10 +5666,10 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
@@ -5696,7 +5696,7 @@
         <v>44</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>10</v>
@@ -5723,7 +5723,7 @@
         <v>11</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U56" s="2" t="s">
         <v>10</v>
@@ -5732,7 +5732,7 @@
         <v>11</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y56" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5741,13 +5741,13 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>14</v>
@@ -5771,7 +5771,7 @@
         <v>44</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>10</v>
@@ -5798,7 +5798,7 @@
         <v>10</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U57" s="2" t="s">
         <v>10</v>
@@ -5807,7 +5807,7 @@
         <v>11</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y57" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5816,11 +5816,11 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C58" s="1" t="s">
         <v>14</v>
       </c>
@@ -5843,10 +5843,10 @@
         <v>10</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>10</v>
@@ -5873,7 +5873,7 @@
         <v>11</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U58" s="2" t="s">
         <v>11</v>
@@ -5882,7 +5882,7 @@
         <v>10</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y58" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5891,11 +5891,11 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C59" s="1" t="s">
         <v>14</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>10</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>14</v>
@@ -5948,7 +5948,7 @@
         <v>10</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U59" s="2" t="s">
         <v>10</v>
@@ -5966,10 +5966,10 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>14</v>
@@ -5996,7 +5996,7 @@
         <v>44</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>10</v>
@@ -6023,7 +6023,7 @@
         <v>10</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U60" s="2" t="s">
         <v>10</v>
@@ -6041,11 +6041,11 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C61" s="1" t="s">
         <v>14</v>
       </c>
@@ -6068,10 +6068,10 @@
         <v>10</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>11</v>
@@ -6098,7 +6098,7 @@
         <v>10</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U61" s="2" t="s">
         <v>10</v>
@@ -6107,7 +6107,7 @@
         <v>10</v>
       </c>
       <c r="W61" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y61" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6116,13 +6116,13 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>14</v>
@@ -6146,7 +6146,7 @@
         <v>59</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>11</v>
@@ -6173,7 +6173,7 @@
         <v>11</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U62" s="2" t="s">
         <v>10</v>
@@ -6191,14 +6191,14 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="D63" s="1" t="s">
         <v>14</v>
       </c>
@@ -6218,10 +6218,10 @@
         <v>10</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>11</v>
@@ -6248,7 +6248,7 @@
         <v>10</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U63" s="2" t="s">
         <v>10</v>
@@ -6257,7 +6257,7 @@
         <v>10</v>
       </c>
       <c r="W63" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y63" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6266,11 +6266,11 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C64" s="1" t="s">
         <v>14</v>
       </c>
@@ -6293,10 +6293,10 @@
         <v>10</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>11</v>
@@ -6332,7 +6332,7 @@
         <v>10</v>
       </c>
       <c r="W64" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y64" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6341,10 +6341,10 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>14</v>
@@ -6371,7 +6371,7 @@
         <v>44</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>10</v>
@@ -6398,7 +6398,7 @@
         <v>11</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U65" s="2" t="s">
         <v>10</v>
@@ -6407,7 +6407,7 @@
         <v>11</v>
       </c>
       <c r="W65" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y65" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6416,11 +6416,11 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C66" s="1" t="s">
         <v>14</v>
       </c>
@@ -6443,10 +6443,10 @@
         <v>11</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>10</v>
@@ -6473,7 +6473,7 @@
         <v>11</v>
       </c>
       <c r="T66" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U66" s="2" t="s">
         <v>11</v>
@@ -6491,11 +6491,11 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C67" s="1" t="s">
         <v>14</v>
       </c>
@@ -6518,10 +6518,10 @@
         <v>10</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>11</v>
@@ -6548,7 +6548,7 @@
         <v>10</v>
       </c>
       <c r="T67" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U67" s="2" t="s">
         <v>11</v>
@@ -6566,11 +6566,11 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C68" s="1" t="s">
         <v>14</v>
       </c>
@@ -6593,10 +6593,10 @@
         <v>10</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>10</v>
@@ -6623,7 +6623,7 @@
         <v>10</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U68" s="2" t="s">
         <v>10</v>
@@ -6632,7 +6632,7 @@
         <v>10</v>
       </c>
       <c r="W68" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y68" s="3" t="str">
         <f t="shared" ref="Y68:Y105" si="1">CONCATENATE("(",$A68,",",$B68,",",$C68,",",$D68,",",$E68,",",$F68,",",$G68,",",$H68,",",$I68,",",$J68,",",$K68,",",$L68,",",$M68,",",$N68,",",$O68,",",$P68,",",$Q68,",",$R68,",",$S68,",",$T68,",",$U68,",",$V68,",",$W68,"),")</f>
@@ -6641,11 +6641,11 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C69" s="1" t="s">
         <v>14</v>
       </c>
@@ -6668,10 +6668,10 @@
         <v>10</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>11</v>
@@ -6698,7 +6698,7 @@
         <v>10</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U69" s="2" t="s">
         <v>10</v>
@@ -6707,7 +6707,7 @@
         <v>11</v>
       </c>
       <c r="W69" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y69" s="3" t="str">
         <f t="shared" si="1"/>
@@ -6716,11 +6716,11 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C70" s="1" t="s">
         <v>14</v>
       </c>
@@ -6743,10 +6743,10 @@
         <v>10</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>10</v>
@@ -6773,7 +6773,7 @@
         <v>11</v>
       </c>
       <c r="T70" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U70" s="2" t="s">
         <v>10</v>
@@ -6791,11 +6791,11 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C71" s="1" t="s">
         <v>14</v>
       </c>
@@ -6818,10 +6818,10 @@
         <v>10</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>11</v>
@@ -6848,7 +6848,7 @@
         <v>10</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U71" s="2" t="s">
         <v>10</v>
@@ -6866,11 +6866,11 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C72" s="1" t="s">
         <v>14</v>
       </c>
@@ -6893,10 +6893,10 @@
         <v>10</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>11</v>
@@ -6941,11 +6941,11 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>14</v>
       </c>
@@ -6968,10 +6968,10 @@
         <v>10</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>10</v>
@@ -7016,14 +7016,14 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D74" s="1" t="s">
         <v>14</v>
       </c>
@@ -7043,10 +7043,10 @@
         <v>10</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>11</v>
@@ -7055,7 +7055,7 @@
         <v>12</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>10</v>
@@ -7091,10 +7091,10 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>14</v>
@@ -7121,7 +7121,7 @@
         <v>44</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>11</v>
@@ -7148,7 +7148,7 @@
         <v>10</v>
       </c>
       <c r="T75" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U75" s="2" t="s">
         <v>10</v>
@@ -7157,7 +7157,7 @@
         <v>11</v>
       </c>
       <c r="W75" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y75" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7166,14 +7166,14 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="D76" s="1" t="s">
         <v>14</v>
       </c>
@@ -7193,10 +7193,10 @@
         <v>10</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>11</v>
@@ -7241,11 +7241,11 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="C77" s="1" t="s">
         <v>14</v>
       </c>
@@ -7268,10 +7268,10 @@
         <v>10</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>11</v>
@@ -7298,7 +7298,7 @@
         <v>11</v>
       </c>
       <c r="T77" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U77" s="2" t="s">
         <v>10</v>
@@ -7307,7 +7307,7 @@
         <v>10</v>
       </c>
       <c r="W77" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y77" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7316,11 +7316,11 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
@@ -7343,10 +7343,10 @@
         <v>10</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>10</v>
@@ -7373,7 +7373,7 @@
         <v>10</v>
       </c>
       <c r="T78" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U78" s="2" t="s">
         <v>10</v>
@@ -7382,7 +7382,7 @@
         <v>11</v>
       </c>
       <c r="W78" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y78" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7391,11 +7391,11 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>14</v>
       </c>
@@ -7418,10 +7418,10 @@
         <v>10</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>11</v>
@@ -7448,7 +7448,7 @@
         <v>11</v>
       </c>
       <c r="T79" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U79" s="2" t="s">
         <v>10</v>
@@ -7457,7 +7457,7 @@
         <v>11</v>
       </c>
       <c r="W79" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y79" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7466,14 +7466,14 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
       </c>
@@ -7493,10 +7493,10 @@
         <v>10</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>11</v>
@@ -7541,11 +7541,11 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
@@ -7568,10 +7568,10 @@
         <v>10</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>11</v>
@@ -7598,7 +7598,7 @@
         <v>10</v>
       </c>
       <c r="T81" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U81" s="2" t="s">
         <v>10</v>
@@ -7616,11 +7616,11 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C82" s="1" t="s">
         <v>14</v>
       </c>
@@ -7643,10 +7643,10 @@
         <v>10</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>10</v>
@@ -7673,7 +7673,7 @@
         <v>10</v>
       </c>
       <c r="T82" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U82" s="2" t="s">
         <v>10</v>
@@ -7682,7 +7682,7 @@
         <v>10</v>
       </c>
       <c r="W82" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y82" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7691,11 +7691,11 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C83" s="1" t="s">
         <v>14</v>
       </c>
@@ -7718,10 +7718,10 @@
         <v>10</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>10</v>
@@ -7748,7 +7748,7 @@
         <v>11</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U83" s="2" t="s">
         <v>10</v>
@@ -7766,10 +7766,10 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>14</v>
@@ -7796,7 +7796,7 @@
         <v>59</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>10</v>
@@ -7841,10 +7841,10 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>14</v>
@@ -7898,7 +7898,7 @@
         <v>10</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U85" s="2" t="s">
         <v>10</v>
@@ -7916,10 +7916,10 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>14</v>
@@ -7973,7 +7973,7 @@
         <v>10</v>
       </c>
       <c r="T86" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U86" s="2" t="s">
         <v>10</v>
@@ -7991,10 +7991,10 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>14</v>
@@ -8048,7 +8048,7 @@
         <v>10</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U87" s="2" t="s">
         <v>10</v>
@@ -8066,10 +8066,10 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>14</v>
@@ -8123,7 +8123,7 @@
         <v>10</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U88" s="2" t="s">
         <v>10</v>
@@ -8141,10 +8141,10 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>14</v>
@@ -8171,7 +8171,7 @@
         <v>59</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>10</v>
@@ -8198,7 +8198,7 @@
         <v>10</v>
       </c>
       <c r="T89" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U89" s="2" t="s">
         <v>10</v>
@@ -8216,10 +8216,10 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>14</v>
@@ -8255,7 +8255,7 @@
         <v>12</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>10</v>
@@ -8291,10 +8291,10 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>14</v>
@@ -8321,7 +8321,7 @@
         <v>59</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>10</v>
@@ -8348,7 +8348,7 @@
         <v>10</v>
       </c>
       <c r="T91" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U91" s="2" t="s">
         <v>11</v>
@@ -8366,10 +8366,10 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>14</v>
@@ -8396,7 +8396,7 @@
         <v>59</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>10</v>
@@ -8423,7 +8423,7 @@
         <v>10</v>
       </c>
       <c r="T92" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U92" s="2" t="s">
         <v>10</v>
@@ -8441,10 +8441,10 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>14</v>
@@ -8471,7 +8471,7 @@
         <v>59</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>10</v>
@@ -8516,10 +8516,10 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>14</v>
@@ -8546,7 +8546,7 @@
         <v>59</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>10</v>
@@ -8582,7 +8582,7 @@
         <v>10</v>
       </c>
       <c r="W94" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y94" s="3" t="str">
         <f t="shared" si="1"/>
@@ -8591,10 +8591,10 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>14</v>
@@ -8621,7 +8621,7 @@
         <v>59</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>10</v>
@@ -8666,10 +8666,10 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>14</v>
@@ -8696,7 +8696,7 @@
         <v>59</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>10</v>
@@ -8705,7 +8705,7 @@
         <v>12</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>11</v>
@@ -8723,7 +8723,7 @@
         <v>10</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U96" s="2" t="s">
         <v>10</v>
@@ -8741,10 +8741,10 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>14</v>
@@ -8771,7 +8771,7 @@
         <v>59</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>10</v>
@@ -8798,7 +8798,7 @@
         <v>10</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U97" s="2" t="s">
         <v>10</v>
@@ -8816,10 +8816,10 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>14</v>
@@ -8846,7 +8846,7 @@
         <v>59</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>10</v>
@@ -8873,7 +8873,7 @@
         <v>10</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U98" s="2" t="s">
         <v>10</v>
@@ -8891,13 +8891,13 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>14</v>
@@ -8921,7 +8921,7 @@
         <v>59</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>10</v>
@@ -8966,10 +8966,10 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>14</v>
@@ -8996,7 +8996,7 @@
         <v>59</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>10</v>
@@ -9023,7 +9023,7 @@
         <v>10</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U100" s="2" t="s">
         <v>10</v>
@@ -9032,7 +9032,7 @@
         <v>10</v>
       </c>
       <c r="W100" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y100" s="3" t="str">
         <f t="shared" si="1"/>
@@ -9041,10 +9041,10 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>14</v>
@@ -9071,7 +9071,7 @@
         <v>44</v>
       </c>
       <c r="K101" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>11</v>
@@ -9116,14 +9116,14 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="D102" s="1" t="s">
         <v>14</v>
       </c>
@@ -9143,10 +9143,10 @@
         <v>10</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K102" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>11</v>
@@ -9173,7 +9173,7 @@
         <v>10</v>
       </c>
       <c r="T102" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U102" s="2" t="s">
         <v>10</v>
@@ -9182,7 +9182,7 @@
         <v>10</v>
       </c>
       <c r="W102" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y102" s="3" t="str">
         <f t="shared" si="1"/>
@@ -9191,10 +9191,10 @@
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>14</v>
@@ -9221,7 +9221,7 @@
         <v>44</v>
       </c>
       <c r="K103" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>11</v>
@@ -9248,7 +9248,7 @@
         <v>10</v>
       </c>
       <c r="T103" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="U103" s="2" t="s">
         <v>10</v>
@@ -9266,11 +9266,11 @@
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="C104" s="1" t="s">
         <v>14</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>11</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>14</v>
@@ -9323,7 +9323,7 @@
         <v>10</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>10</v>
@@ -9341,11 +9341,11 @@
     </row>
     <row r="105" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="C105" s="1" t="s">
         <v>14</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>10</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>14</v>
@@ -9453,21 +9453,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9559,26 +9559,26 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
@@ -9701,18 +9701,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9741,18 +9741,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9781,18 +9781,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9821,18 +9821,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9861,18 +9861,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9901,18 +9901,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9941,18 +9941,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -9981,18 +9981,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10021,18 +10021,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10061,18 +10061,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10101,18 +10101,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10141,18 +10141,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10181,18 +10181,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -10227,21 +10227,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E2" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -10249,10 +10249,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
@@ -10261,13 +10261,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" ref="E4:E5" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
@@ -10279,10 +10279,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -10322,27 +10322,27 @@
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -10354,7 +10354,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -10366,7 +10366,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -10378,7 +10378,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -10390,7 +10390,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -10402,7 +10402,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -10414,7 +10414,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -10426,7 +10426,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -10438,7 +10438,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -10450,7 +10450,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -10462,7 +10462,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -10474,7 +10474,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -10486,7 +10486,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -10498,7 +10498,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -10510,7 +10510,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -10522,7 +10522,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -10534,7 +10534,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -10546,7 +10546,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -10558,7 +10558,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -10570,7 +10570,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -10582,7 +10582,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -10594,7 +10594,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -10606,7 +10606,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -10618,7 +10618,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -10630,7 +10630,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -10681,18 +10681,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Datensammlung, UC 5
</commit_message>
<xml_diff>
--- a/Simpsons.xlsx
+++ b/Simpsons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="437">
   <si>
     <t>INT</t>
   </si>
@@ -914,9 +914,6 @@
     <t>'bar'</t>
   </si>
   <si>
-    <t>'major'</t>
-  </si>
-  <si>
     <t>'farmer'</t>
   </si>
   <si>
@@ -1043,61 +1040,310 @@
     <t>DROP TABLE IF EXISTS Simpsons; CREATE TABLE Simpsons(ID INT PRIMARY KEY, name VARCHAR, nickname VARCHAR, description_en VARCHAR, description_de VARCHAR, male BOOL, FOREIGN KEY (male) REFERENCES public.MALE_QUESTIONS(ID), human BOOL, FOREIGN KEY (human) REFERENCES public.HUMAN_QUESTIONS(ID), alive BOOL, FOREIGN KEY (alive) REFERENCES public.ALIVE_QUESTIONS(ID), simpson BOOL, FOREIGN KEY (simpson) REFERENCES public.SIMPSON_QUESTIONS(ID), age VARCHAR, FOREIGN KEY (age) REFERENCES public.AGE_QUESTIONS(ID), job VARCHAR, FOREIGN KEY (job) REFERENCES public.JOB_QUESTIONS(ID), famous BOOL, FOREIGN KEY (famous) REFERENCES public.FAMOUS_QUESTIONS(ID), skincolor VARCHAR, FOREIGN KEY (skincolor) REFERENCES public.SKINCOLOR_QUESTIONS(ID), haircolor VARCHAR, FOREIGN KEY (haircolor) REFERENCES public.HAIRCOLOR_QUESTIONS(ID), religous BOOL, FOREIGN KEY (religous) REFERENCES public.RELIGOUS_QUESTIONS(ID), smokes BOOL, FOREIGN KEY (smokes) REFERENCES public.SMOKES_QUESTIONS(ID), homosexual BOOL, FOREIGN KEY (homosexual) REFERENCES public.HOMOSEXUAL_QUESTIONS(ID), american BOOL, FOREIGN KEY (american) REFERENCES public.AMERICAN_QUESTIONS(ID), married BOOL, FOREIGN KEY (married) REFERENCES public.MARRIED_QUESTIONS(ID), character VARCHAR, FOREIGN KEY (character) REFERENCES public.CHARACTER_QUESTIONS(ID), moes_bar BOOL, FOREIGN KEY (moes_bar) REFERENCES public.MOESBAR_QUESTIONS(ID), fat BOOL, FOREIGN KEY (fat) REFERENCES public.FAT_QUESTIONS(ID), wearings VARCHAR, FOREIGN KEY (wearings) REFERENCES public.WEARINGS_QUESTIONS(ID));</t>
   </si>
   <si>
-    <t>DROP TABLE IF EXISTS MALE_QUESTIONS; CREATE TABLE MALE_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS HUMAN_QUESTIONS; CREATE TABLE HUMAN_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS ALIVE_QUESTIONS; CREATE TABLE ALIVE_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS SIMPSON_QUESTIONS; CREATE TABLE SIMPSON_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
     <t>DROP TABLE IF EXISTS AGE_QUESTIONS; CREATE TABLE AGE_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
     <t>DROP TABLE IF EXISTS JOB_QUESTIONS; CREATE TABLE JOB_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
-    <t>DROP TABLE IF EXISTS FAMOUS_QUESTIONS; CREATE TABLE FAMOUS_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
     <t>DROP TABLE IF EXISTS SKINCOLOR_QUESTIONS; CREATE TABLE SKINCOLOR_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
     <t>DROP TABLE IF EXISTS HAIRCOLOR_QUESTIONS; CREATE TABLE HAIRCOLOR_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
-    <t>DROP TABLE IF EXISTS RELIGOUS_QUESTIONS; CREATE TABLE RELIGOUS_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS SMOKES_QUESTIONS; CREATE TABLE SMOKES_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS HOMOSEXUAL_QUESTIONS; CREATE TABLE HOMOSEXUAL_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS AMERICAN_QUESTIONS; CREATE TABLE AMERICAN_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS MARRIED_QUESTIONS; CREATE TABLE MARRIED_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
     <t>DROP TABLE IF EXISTS CHARACTER_QUESTIONS; CREATE TABLE CHARACTER_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
-    <t>DROP TABLE IF EXISTS MOESBAR_QUESTIONS; CREATE TABLE MOESBAR_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
-    <t>DROP TABLE IF EXISTS FAT_QUESTIONS; CREATE TABLE FAT_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
-  </si>
-  <si>
     <t>DROP TABLE IF EXISTS WEARINGS_QUESTIONS; CREATE TABLE WEARINGS_QUESTIONS( ID VARCHAR PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
   </si>
   <si>
     <t>'Barry Huffman'</t>
+  </si>
+  <si>
+    <t>Insert Into MALE_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur in der Fernsehbranche?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur in einem Restaurant?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Krimineller?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur als Assistent?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur eine Nanny?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur für die Kirche?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur für die Feuerwehr?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Maskotschen?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur in der Führersteinstelle?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur arbeitslos?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur im Atomkraftwerk?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur Einzelhändler?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur eine Hausfrau?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Farmer?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur in einer Bar?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Sportler?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Wissenschaftler?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur als Bürgermeister?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur für die Presse tätig?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Rentner?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur Schüler/Student?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur bei der Polizei?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Doktor?</t>
+  </si>
+  <si>
+    <t>Ist dein Charakter männlich?</t>
+  </si>
+  <si>
+    <t>Ist deine Charakter weiblich?</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS MALE_QUESTIONS; CREATE TABLE MALE_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS HUMAN_QUESTIONS; CREATE TABLE HUMAN_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS ALIVE_QUESTIONS; CREATE TABLE ALIVE_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS SIMPSON_QUESTIONS; CREATE TABLE SIMPSON_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS FAMOUS_QUESTIONS; CREATE TABLE FAMOUS_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS RELIGOUS_QUESTIONS; CREATE TABLE RELIGOUS_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS SMOKES_QUESTIONS; CREATE TABLE SMOKES_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS HOMOSEXUAL_QUESTIONS; CREATE TABLE HOMOSEXUAL_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS AMERICAN_QUESTIONS; CREATE TABLE AMERICAN_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS MARRIED_QUESTIONS; CREATE TABLE MARRIED_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS MOESBAR_QUESTIONS; CREATE TABLE MOESBAR_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>DROP TABLE IF EXISTS FAT_QUESTIONS; CREATE TABLE FAT_QUESTIONS( ID BOOL PRIMARY KEY, q1_en VARCHAR, q1_de VARCHAR);</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur als Flugassistent?</t>
+  </si>
+  <si>
+    <t>Insert Into FAMOUS_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into HUMAN_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into ALIVE_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into SIMPSON_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into SKINCOLOR_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into HAIRCOLOR_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into RELIGOUS_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into SMOKES_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into HOMOSEXUAL_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into AMERICAN_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into MARRIED_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into CHARACTER_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into MOESBAR_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into FAT_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Insert Into WEARINGS_QUESTIONS values</t>
+  </si>
+  <si>
+    <t>Ist deine Figur ein Mensch?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur kein Mensch?</t>
+  </si>
+  <si>
+    <t>Lebt deine Figur?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur schon gestorben?</t>
+  </si>
+  <si>
+    <t>Is your character male?</t>
+  </si>
+  <si>
+    <t>Is your character female?</t>
+  </si>
+  <si>
+    <t>Is your character human?</t>
+  </si>
+  <si>
+    <t>Is your character non-human?</t>
+  </si>
+  <si>
+    <t>Is your character alive?</t>
+  </si>
+  <si>
+    <t>Is your character dead?</t>
+  </si>
+  <si>
+    <t>Ist deine Figur verwandt mit den Simpsons?</t>
+  </si>
+  <si>
+    <t>Is your character related with the simpsons?</t>
+  </si>
+  <si>
+    <t>Steht deine Figur auserhalb der Simpson Familie?</t>
+  </si>
+  <si>
+    <t>Is your character outside of the simpson family?</t>
+  </si>
+  <si>
+    <t>Is your character a criminal?</t>
+  </si>
+  <si>
+    <t>Is your character a Nanny?</t>
+  </si>
+  <si>
+    <t>Is your character unemployed?</t>
+  </si>
+  <si>
+    <t>Is your character a housewife?</t>
+  </si>
+  <si>
+    <t>Is your character a Farmer?</t>
+  </si>
+  <si>
+    <t>Is your character an athlete?</t>
+  </si>
+  <si>
+    <t>Is your character a scientist?</t>
+  </si>
+  <si>
+    <t>Is your character a pensioner?</t>
+  </si>
+  <si>
+    <t>Is your character a Doctor?</t>
+  </si>
+  <si>
+    <t>Does your character work in the television industry?</t>
+  </si>
+  <si>
+    <t>Does your character work in a restaurant?</t>
+  </si>
+  <si>
+    <t>is your character an assistant?</t>
+  </si>
+  <si>
+    <t>Does your character work for the fire department?</t>
+  </si>
+  <si>
+    <t>Does your character work for the Church?</t>
+  </si>
+  <si>
+    <t>Is your character a mascot?</t>
+  </si>
+  <si>
+    <t>Does your character work in the driving license office?</t>
+  </si>
+  <si>
+    <t>Does your character work in the nuclear power plant?</t>
+  </si>
+  <si>
+    <t>Is your character a retailer?</t>
+  </si>
+  <si>
+    <t>Arbeitet deine Figur in der Schule?</t>
+  </si>
+  <si>
+    <t>Does your character work in a bar?</t>
+  </si>
+  <si>
+    <t>Does your character work at school?</t>
+  </si>
+  <si>
+    <t>Does your character work as mayor?</t>
+  </si>
+  <si>
+    <t>'mayor'</t>
+  </si>
+  <si>
+    <t>Is your character working for the press?</t>
+  </si>
+  <si>
+    <t>Is your character a student?</t>
+  </si>
+  <si>
+    <t>Does your character work as a flight assistant?</t>
+  </si>
+  <si>
+    <t>Does your character work for the police?</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1700,64 +1946,64 @@
         <v>5</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>309</v>
-      </c>
       <c r="K2" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="S2" s="22" t="s">
+      <c r="U2" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="V2" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="W2" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="V2" s="22" t="s">
-        <v>318</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>324</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>6</v>
@@ -1792,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
@@ -1867,10 +2113,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>293</v>
+        <v>432</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>10</v>
@@ -1910,7 +2156,7 @@
       </c>
       <c r="Y4" s="3" t="str">
         <f t="shared" ref="Y4:Y67" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,",",$D4,",",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,",",$U4,",",$V4,",",$W4,"),")</f>
-        <v>(02,'Martha Quimby',null,null,null,false,true,true,false,'adult','major',false,'yellow','black',false,false,false,true,true,'sane',false,false,'hat'),</v>
+        <v>(02,'Martha Quimby',null,null,null,false,true,true,false,'adult','mayor',false,'yellow','black',false,false,false,true,true,'sane',false,false,'hat'),</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1942,7 +2188,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>281</v>
@@ -2017,7 +2263,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>285</v>
@@ -2092,7 +2338,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>282</v>
@@ -2167,7 +2413,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>280</v>
@@ -2242,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>280</v>
@@ -2317,7 +2563,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>283</v>
@@ -2392,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>283</v>
@@ -2467,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>283</v>
@@ -2542,7 +2788,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>280</v>
@@ -2692,10 +2938,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>10</v>
@@ -2767,10 +3013,10 @@
         <v>11</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>10</v>
@@ -2842,7 +3088,7 @@
         <v>11</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>280</v>
@@ -2992,10 +3238,10 @@
         <v>10</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>10</v>
@@ -3067,7 +3313,7 @@
         <v>10</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>280</v>
@@ -3145,7 +3391,7 @@
         <v>59</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>10</v>
@@ -3220,7 +3466,7 @@
         <v>59</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>10</v>
@@ -3445,7 +3691,7 @@
         <v>59</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>10</v>
@@ -3517,7 +3763,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>14</v>
@@ -3668,7 +3914,7 @@
         <v>10</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>284</v>
@@ -3719,7 +3965,7 @@
         <v>79</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>80</v>
@@ -3743,7 +3989,7 @@
         <v>10</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>285</v>
@@ -3818,7 +4064,7 @@
         <v>10</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>286</v>
@@ -3968,10 +4214,10 @@
         <v>11</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>10</v>
@@ -4043,7 +4289,7 @@
         <v>10</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>287</v>
@@ -4193,7 +4439,7 @@
         <v>10</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>288</v>
@@ -4343,7 +4589,7 @@
         <v>10</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>287</v>
@@ -4418,7 +4664,7 @@
         <v>10</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>282</v>
@@ -4493,7 +4739,7 @@
         <v>10</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>291</v>
@@ -4568,7 +4814,7 @@
         <v>10</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>289</v>
@@ -4643,7 +4889,7 @@
         <v>10</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>288</v>
@@ -4718,7 +4964,7 @@
         <v>10</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>287</v>
@@ -4793,7 +5039,7 @@
         <v>10</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>284</v>
@@ -4868,7 +5114,7 @@
         <v>10</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>284</v>
@@ -4943,7 +5189,7 @@
         <v>10</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>284</v>
@@ -5018,7 +5264,7 @@
         <v>10</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>290</v>
@@ -5243,7 +5489,7 @@
         <v>10</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K50" s="5" t="s">
         <v>283</v>
@@ -5318,7 +5564,7 @@
         <v>10</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>288</v>
@@ -5393,7 +5639,7 @@
         <v>10</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>282</v>
@@ -5468,7 +5714,7 @@
         <v>10</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K53" s="5" t="s">
         <v>283</v>
@@ -5543,7 +5789,7 @@
         <v>10</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>283</v>
@@ -5618,7 +5864,7 @@
         <v>11</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K55" s="5" t="s">
         <v>284</v>
@@ -5843,7 +6089,7 @@
         <v>10</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>284</v>
@@ -5918,7 +6164,7 @@
         <v>10</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>14</v>
@@ -6068,7 +6314,7 @@
         <v>10</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>287</v>
@@ -6146,7 +6392,7 @@
         <v>59</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>293</v>
+        <v>432</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>11</v>
@@ -6186,7 +6432,7 @@
       </c>
       <c r="Y62" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>(59,'Joseph Quimby','Joe',null,null,true,true,true,false,'young','major',true,'yellow','brown',false,false,false,true,true,'corrupt',false,true,null),</v>
+        <v>(59,'Joseph Quimby','Joe',null,null,true,true,true,false,'young','mayor',true,'yellow','brown',false,false,false,true,true,'corrupt',false,true,null),</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
@@ -6218,7 +6464,7 @@
         <v>10</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>290</v>
@@ -6293,10 +6539,10 @@
         <v>10</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>11</v>
@@ -6443,7 +6689,7 @@
         <v>11</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>288</v>
@@ -6518,7 +6764,7 @@
         <v>10</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>283</v>
@@ -6593,7 +6839,7 @@
         <v>10</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>288</v>
@@ -6668,7 +6914,7 @@
         <v>10</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>286</v>
@@ -6743,10 +6989,10 @@
         <v>10</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>10</v>
@@ -6818,7 +7064,7 @@
         <v>10</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>292</v>
@@ -6893,10 +7139,10 @@
         <v>10</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>11</v>
@@ -6968,7 +7214,7 @@
         <v>10</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>289</v>
@@ -7043,10 +7289,10 @@
         <v>10</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>11</v>
@@ -7193,10 +7439,10 @@
         <v>10</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>11</v>
@@ -7268,7 +7514,7 @@
         <v>10</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K77" s="5" t="s">
         <v>287</v>
@@ -7343,10 +7589,10 @@
         <v>10</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>10</v>
@@ -7418,7 +7664,7 @@
         <v>10</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K79" s="5" t="s">
         <v>286</v>
@@ -7493,10 +7739,10 @@
         <v>10</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>11</v>
@@ -7568,7 +7814,7 @@
         <v>10</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K81" s="5" t="s">
         <v>287</v>
@@ -7643,7 +7889,7 @@
         <v>10</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K82" s="5" t="s">
         <v>284</v>
@@ -7718,7 +7964,7 @@
         <v>10</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K83" s="5" t="s">
         <v>284</v>
@@ -7796,7 +8042,7 @@
         <v>59</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>10</v>
@@ -8171,7 +8417,7 @@
         <v>59</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>10</v>
@@ -8321,7 +8567,7 @@
         <v>59</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>10</v>
@@ -8396,7 +8642,7 @@
         <v>59</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>10</v>
@@ -8471,7 +8717,7 @@
         <v>59</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>10</v>
@@ -8546,7 +8792,7 @@
         <v>59</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>10</v>
@@ -8621,7 +8867,7 @@
         <v>59</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>10</v>
@@ -8696,7 +8942,7 @@
         <v>59</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>10</v>
@@ -8771,7 +9017,7 @@
         <v>59</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>10</v>
@@ -8846,7 +9092,7 @@
         <v>59</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>10</v>
@@ -8921,7 +9167,7 @@
         <v>59</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>10</v>
@@ -8996,7 +9242,7 @@
         <v>59</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>10</v>
@@ -9143,7 +9389,7 @@
         <v>10</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K102" s="5" t="s">
         <v>287</v>
@@ -9293,7 +9539,7 @@
         <v>11</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>14</v>
@@ -9368,7 +9614,7 @@
         <v>10</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>14</v>
@@ -9437,7 +9683,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9453,21 +9699,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9543,7 +9789,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9559,21 +9805,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9682,10 +9928,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9701,18 +9947,33 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>345</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
       </c>
     </row>
   </sheetData>
@@ -9722,10 +9983,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9741,18 +10002,33 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>346</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
       </c>
     </row>
   </sheetData>
@@ -9762,287 +10038,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -10061,18 +10057,436 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
       <c r="C2" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(true,Is your character male?,Ist dein Charakter männlich?),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(false,Is your character female?,Ist deine Charakter weiblich?),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(,,),</v>
       </c>
     </row>
   </sheetData>
@@ -10082,17 +10496,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -10101,18 +10515,51 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>337</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(true,Is your character human?,Ist deine Figur ein Mensch?),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(false,Is your character non-human?,Ist deine Figur kein Mensch?),</v>
       </c>
     </row>
   </sheetData>
@@ -10122,17 +10569,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -10141,18 +10588,51 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>338</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(true,Is your character alive?,Lebt deine Figur?),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(false,Is your character dead?,Ist deine Figur schon gestorben?),</v>
       </c>
     </row>
   </sheetData>
@@ -10162,17 +10642,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -10181,18 +10661,51 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(true,Is your character related with the simpsons?,Ist deine Figur verwandt mit den Simpsons?),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(false,Is your character outside of the simpson family?,Steht deine Figur auserhalb der Simpson Familie?),</v>
       </c>
     </row>
   </sheetData>
@@ -10205,7 +10718,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10227,21 +10740,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E2" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -10249,10 +10762,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
@@ -10261,13 +10774,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" ref="E4:E5" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
@@ -10279,10 +10792,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -10300,14 +10813,15 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="1025" width="10.7109375"/>
+    <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -10322,322 +10836,422 @@
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>343</v>
+      </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3" t="str">
         <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
-        <v>('tv',,),</v>
+        <v>('tv',Does your character work in the television industry?,Arbeitet deine Figur in der Fernsehbranche?),</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>344</v>
+      </c>
       <c r="D4" s="19"/>
       <c r="E4" s="3" t="str">
         <f t="shared" ref="E4:E27" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
-        <v>('restaurant',,),</v>
+        <v>('restaurant',Does your character work in a restaurant?,Arbeitet deine Figur in einem Restaurant?),</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+        <v>295</v>
+      </c>
+      <c r="B5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>345</v>
+      </c>
       <c r="D5" s="19"/>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('criminal',,),</v>
+        <v>('criminal',Is your character a criminal?,Ist deine Figur ein Krimineller?),</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+        <v>300</v>
+      </c>
+      <c r="B6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>346</v>
+      </c>
       <c r="D6" s="19"/>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('assistent',,),</v>
+        <v>('assistent',is your character an assistant?,Arbeitet deine Figur als Assistent?),</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
+        <v>297</v>
+      </c>
+      <c r="B7" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>347</v>
+      </c>
       <c r="D7" s="19"/>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('nanny',,),</v>
+        <v>('nanny',Is your character a Nanny?,Ist deine Figur eine Nanny?),</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>348</v>
+      </c>
       <c r="D8" s="19"/>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('church',,),</v>
+        <v>('church',Does your character work for the Church?,Arbeitet deine Figur für die Kirche?),</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" t="s">
+        <v>422</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="D9" s="19"/>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('firefighter',,),</v>
+        <v>('firefighter',Does your character work for the fire department?,Arbeitet deine Figur für die Feuerwehr?),</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>350</v>
+      </c>
       <c r="D10" s="19"/>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('mascot',,),</v>
+        <v>('mascot',Is your character a mascot?,Ist deine Figur ein Maskotschen?),</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+        <v>318</v>
+      </c>
+      <c r="B11" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>351</v>
+      </c>
       <c r="D11" s="19"/>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('driving license office',,),</v>
+        <v>('driving license office',Does your character work in the driving license office?,Arbeitet deine Figur in der Führersteinstelle?),</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>352</v>
+      </c>
       <c r="D12" s="19"/>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('unemployed',,),</v>
+        <v>('unemployed',Is your character unemployed?,Ist deine Figur arbeitslos?),</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" t="s">
+        <v>426</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>353</v>
+      </c>
       <c r="D13" s="19"/>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('akw',,),</v>
+        <v>('akw',Does your character work in the nuclear power plant?,Arbeitet deine Figur im Atomkraftwerk?),</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
+      <c r="B14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>354</v>
+      </c>
       <c r="D14" s="19"/>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('retailer',,),</v>
+        <v>('retailer',Is your character a retailer?,Ist deine Figur Einzelhändler?),</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" t="s">
+        <v>413</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>355</v>
+      </c>
       <c r="D15" s="19"/>
       <c r="E15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('wife',,),</v>
+        <v>('wife',Is your character a housewife?,Ist deine Figur eine Hausfrau?),</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>294</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
+        <v>293</v>
+      </c>
+      <c r="B16" t="s">
+        <v>414</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>356</v>
+      </c>
       <c r="D16" s="19"/>
       <c r="E16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('farmer',,),</v>
+        <v>('farmer',Is your character a Farmer?,Ist deine Figur ein Farmer?),</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" t="s">
+        <v>429</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>357</v>
+      </c>
       <c r="D17" s="19"/>
       <c r="E17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('bar',,),</v>
+        <v>('bar',Does your character work in a bar?,Arbeitet deine Figur in einer Bar?),</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="B18" t="s">
+        <v>430</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>428</v>
+      </c>
       <c r="D18" s="19"/>
       <c r="E18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('school',,),</v>
+        <v>('school',Does your character work at school?,Arbeitet deine Figur in der Schule?),</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+        <v>294</v>
+      </c>
+      <c r="B19" t="s">
+        <v>415</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>358</v>
+      </c>
       <c r="D19" s="19"/>
       <c r="E19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('sport',,),</v>
+        <v>('sport',Is your character an athlete?,Ist deine Figur ein Sportler?),</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+      <c r="B20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>359</v>
+      </c>
       <c r="D20" s="19"/>
       <c r="E20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('scientist',,),</v>
+        <v>('scientist',Is your character a scientist?,Ist deine Figur ein Wissenschaftler?),</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+        <v>432</v>
+      </c>
+      <c r="B21" t="s">
+        <v>431</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>360</v>
+      </c>
       <c r="D21" s="19"/>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('major',,),</v>
+        <v>('mayor',Does your character work as mayor?,Arbeitet deine Figur als Bürgermeister?),</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
+        <v>299</v>
+      </c>
+      <c r="B22" t="s">
+        <v>433</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>361</v>
+      </c>
       <c r="D22" s="19"/>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('press',,),</v>
+        <v>('press',Is your character working for the press?,Ist deine Figur für die Presse tätig?),</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+      <c r="B23" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>362</v>
+      </c>
       <c r="D23" s="19"/>
       <c r="E23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('pensioner',,),</v>
+        <v>('pensioner',Is your character a pensioner?,Ist deine Figur ein Rentner?),</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+        <v>298</v>
+      </c>
+      <c r="B24" t="s">
+        <v>434</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>363</v>
+      </c>
       <c r="D24" s="19"/>
       <c r="E24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('student',,),</v>
+        <v>('student',Is your character a student?,Ist deine Figur Schüler/Student?),</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+        <v>301</v>
+      </c>
+      <c r="B25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>380</v>
+      </c>
       <c r="D25" s="19"/>
       <c r="E25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('flightattendant',,),</v>
+        <v>('flightattendant',Does your character work as a flight assistant?,Arbeitet deine Figur als Flugassistent?),</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
+      <c r="B26" t="s">
+        <v>436</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>364</v>
+      </c>
       <c r="D26" s="19"/>
       <c r="E26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('police',,),</v>
+        <v>('police',Does your character work for the police?,Arbeitet deine Figur bei der Polizei?),</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="B27" t="s">
+        <v>418</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>365</v>
+      </c>
       <c r="D27" s="19"/>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>('doctor',,),</v>
+        <v>('doctor',Is your character a Doctor?,Ist deine Figur ein Doktor?),</v>
       </c>
     </row>
   </sheetData>
@@ -10662,10 +11276,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10681,18 +11295,39 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>342</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
+      <c r="E2" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
+        <v>(true,,),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
+        <v>(false,,),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
descriptions done and little change in xlsx
</commit_message>
<xml_diff>
--- a/Simpsons.xlsx
+++ b/Simpsons.xlsx
@@ -557,9 +557,6 @@
     <t>70</t>
   </si>
   <si>
-    <t>'Cecile Terwilliger'</t>
-  </si>
-  <si>
     <t>71</t>
   </si>
   <si>
@@ -1098,6 +1095,9 @@
   </si>
   <si>
     <t>'Barry Huffman'</t>
+  </si>
+  <si>
+    <t>Cecile Terwilliger'</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1700,64 +1700,64 @@
         <v>5</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>309</v>
-      </c>
       <c r="K2" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="S2" s="22" t="s">
+      <c r="U2" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="V2" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="W2" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="V2" s="22" t="s">
-        <v>318</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>324</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>6</v>
@@ -1792,7 +1792,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>14</v>
@@ -1822,7 +1822,7 @@
         <v>10</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>10</v>
@@ -1867,10 +1867,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>10</v>
@@ -1897,7 +1897,7 @@
         <v>11</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>10</v>
@@ -1906,7 +1906,7 @@
         <v>10</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y4" s="3" t="str">
         <f t="shared" ref="Y4:Y67" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,",",$D4,",",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,",",$U4,",",$V4,",",$W4,"),")</f>
@@ -1942,10 +1942,10 @@
         <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>10</v>
@@ -1972,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>10</v>
@@ -1981,7 +1981,7 @@
         <v>10</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2017,10 +2017,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>10</v>
@@ -2047,7 +2047,7 @@
         <v>11</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>10</v>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
@@ -2122,7 +2122,7 @@
         <v>11</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>10</v>
@@ -2167,10 +2167,10 @@
         <v>10</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>10</v>
@@ -2197,7 +2197,7 @@
         <v>11</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>10</v>
@@ -2206,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2242,10 +2242,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>10</v>
@@ -2272,7 +2272,7 @@
         <v>11</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>11</v>
@@ -2317,10 +2317,10 @@
         <v>10</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>10</v>
@@ -2347,7 +2347,7 @@
         <v>10</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>10</v>
@@ -2356,7 +2356,7 @@
         <v>10</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2392,10 +2392,10 @@
         <v>10</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>10</v>
@@ -2422,7 +2422,7 @@
         <v>10</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>10</v>
@@ -2467,10 +2467,10 @@
         <v>10</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>10</v>
@@ -2497,7 +2497,7 @@
         <v>11</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>11</v>
@@ -2542,10 +2542,10 @@
         <v>10</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>11</v>
@@ -2581,7 +2581,7 @@
         <v>10</v>
       </c>
       <c r="W13" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2620,7 +2620,7 @@
         <v>44</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>10</v>
@@ -2647,7 +2647,7 @@
         <v>10</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>10</v>
@@ -2656,7 +2656,7 @@
         <v>10</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2692,10 +2692,10 @@
         <v>11</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>10</v>
@@ -2722,7 +2722,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U15" s="2" t="s">
         <v>10</v>
@@ -2731,7 +2731,7 @@
         <v>11</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2767,10 +2767,10 @@
         <v>11</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>10</v>
@@ -2797,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U16" s="2" t="s">
         <v>10</v>
@@ -2806,7 +2806,7 @@
         <v>11</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2842,10 +2842,10 @@
         <v>11</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>10</v>
@@ -2872,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U17" s="2" t="s">
         <v>10</v>
@@ -2881,7 +2881,7 @@
         <v>10</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2896,7 +2896,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>14</v>
@@ -2920,7 +2920,7 @@
         <v>44</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>10</v>
@@ -2947,7 +2947,7 @@
         <v>10</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>10</v>
@@ -2956,7 +2956,7 @@
         <v>10</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2992,10 +2992,10 @@
         <v>10</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>10</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U19" s="2" t="s">
         <v>10</v>
@@ -3031,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3067,10 +3067,10 @@
         <v>10</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>10</v>
@@ -3097,7 +3097,7 @@
         <v>11</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>10</v>
@@ -3145,7 +3145,7 @@
         <v>59</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>10</v>
@@ -3172,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U21" s="2" t="s">
         <v>10</v>
@@ -3181,7 +3181,7 @@
         <v>10</v>
       </c>
       <c r="W21" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3220,7 +3220,7 @@
         <v>59</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>10</v>
@@ -3247,7 +3247,7 @@
         <v>10</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>10</v>
@@ -3322,7 +3322,7 @@
         <v>10</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U23" s="2" t="s">
         <v>10</v>
@@ -3331,7 +3331,7 @@
         <v>10</v>
       </c>
       <c r="W23" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y23" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3397,7 +3397,7 @@
         <v>10</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U24" s="2" t="s">
         <v>10</v>
@@ -3406,7 +3406,7 @@
         <v>10</v>
       </c>
       <c r="W24" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y24" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3445,7 +3445,7 @@
         <v>59</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>10</v>
@@ -3472,7 +3472,7 @@
         <v>10</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U25" s="2" t="s">
         <v>10</v>
@@ -3481,7 +3481,7 @@
         <v>10</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y25" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3517,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>14</v>
@@ -3622,7 +3622,7 @@
         <v>10</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U27" s="2" t="s">
         <v>10</v>
@@ -3668,10 +3668,10 @@
         <v>10</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>10</v>
@@ -3698,7 +3698,7 @@
         <v>10</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>11</v>
@@ -3719,7 +3719,7 @@
         <v>79</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>80</v>
@@ -3743,10 +3743,10 @@
         <v>10</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>11</v>
@@ -3773,7 +3773,7 @@
         <v>11</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>10</v>
@@ -3782,7 +3782,7 @@
         <v>10</v>
       </c>
       <c r="W30" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y30" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3818,10 +3818,10 @@
         <v>10</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>11</v>
@@ -3848,7 +3848,7 @@
         <v>10</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>10</v>
@@ -3857,7 +3857,7 @@
         <v>10</v>
       </c>
       <c r="W31" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3896,7 +3896,7 @@
         <v>44</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>10</v>
@@ -3923,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>10</v>
@@ -3932,7 +3932,7 @@
         <v>11</v>
       </c>
       <c r="W32" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3968,10 +3968,10 @@
         <v>11</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>10</v>
@@ -3998,7 +3998,7 @@
         <v>11</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U33" s="2" t="s">
         <v>10</v>
@@ -4043,10 +4043,10 @@
         <v>10</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>11</v>
@@ -4073,7 +4073,7 @@
         <v>11</v>
       </c>
       <c r="T34" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>10</v>
@@ -4121,7 +4121,7 @@
         <v>44</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>11</v>
@@ -4193,10 +4193,10 @@
         <v>10</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>10</v>
@@ -4223,7 +4223,7 @@
         <v>10</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U36" s="2" t="s">
         <v>11</v>
@@ -4271,7 +4271,7 @@
         <v>44</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>11</v>
@@ -4298,7 +4298,7 @@
         <v>10</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U37" s="2" t="s">
         <v>10</v>
@@ -4307,7 +4307,7 @@
         <v>10</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y37" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4343,10 +4343,10 @@
         <v>10</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>11</v>
@@ -4373,7 +4373,7 @@
         <v>10</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U38" s="2" t="s">
         <v>10</v>
@@ -4382,7 +4382,7 @@
         <v>11</v>
       </c>
       <c r="W38" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y38" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4418,10 +4418,10 @@
         <v>10</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>10</v>
@@ -4448,7 +4448,7 @@
         <v>11</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U39" s="2" t="s">
         <v>10</v>
@@ -4457,7 +4457,7 @@
         <v>10</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y39" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4493,10 +4493,10 @@
         <v>10</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>10</v>
@@ -4523,7 +4523,7 @@
         <v>10</v>
       </c>
       <c r="T40" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U40" s="2" t="s">
         <v>10</v>
@@ -4532,7 +4532,7 @@
         <v>11</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y40" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4568,10 +4568,10 @@
         <v>10</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>11</v>
@@ -4598,7 +4598,7 @@
         <v>11</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U41" s="2" t="s">
         <v>11</v>
@@ -4607,7 +4607,7 @@
         <v>10</v>
       </c>
       <c r="W41" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y41" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4643,10 +4643,10 @@
         <v>10</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>10</v>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y42" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4718,10 +4718,10 @@
         <v>10</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>11</v>
@@ -4748,7 +4748,7 @@
         <v>10</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>10</v>
@@ -4757,7 +4757,7 @@
         <v>11</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y43" s="3" t="str">
         <f t="shared" si="0"/>
@@ -4793,10 +4793,10 @@
         <v>10</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>10</v>
@@ -4823,7 +4823,7 @@
         <v>11</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U44" s="2" t="s">
         <v>11</v>
@@ -4868,10 +4868,10 @@
         <v>10</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>10</v>
@@ -4898,7 +4898,7 @@
         <v>10</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U45" s="2" t="s">
         <v>10</v>
@@ -4943,10 +4943,10 @@
         <v>10</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>10</v>
@@ -4973,7 +4973,7 @@
         <v>10</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U46" s="2" t="s">
         <v>10</v>
@@ -5018,10 +5018,10 @@
         <v>10</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>11</v>
@@ -5048,7 +5048,7 @@
         <v>11</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>10</v>
@@ -5096,7 +5096,7 @@
         <v>44</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>11</v>
@@ -5123,7 +5123,7 @@
         <v>10</v>
       </c>
       <c r="T48" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U48" s="2" t="s">
         <v>10</v>
@@ -5171,7 +5171,7 @@
         <v>44</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>11</v>
@@ -5198,7 +5198,7 @@
         <v>10</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U49" s="2" t="s">
         <v>10</v>
@@ -5207,7 +5207,7 @@
         <v>10</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y49" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5243,10 +5243,10 @@
         <v>10</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>10</v>
@@ -5273,7 +5273,7 @@
         <v>10</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U50" s="2" t="s">
         <v>10</v>
@@ -5318,10 +5318,10 @@
         <v>10</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>10</v>
@@ -5348,7 +5348,7 @@
         <v>10</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U51" s="2" t="s">
         <v>11</v>
@@ -5393,10 +5393,10 @@
         <v>10</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>11</v>
@@ -5423,7 +5423,7 @@
         <v>11</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U52" s="2" t="s">
         <v>10</v>
@@ -5468,10 +5468,10 @@
         <v>10</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>10</v>
@@ -5498,7 +5498,7 @@
         <v>10</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U53" s="2" t="s">
         <v>10</v>
@@ -5507,7 +5507,7 @@
         <v>10</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y53" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5543,10 +5543,10 @@
         <v>10</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>10</v>
@@ -5573,7 +5573,7 @@
         <v>10</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U54" s="2" t="s">
         <v>10</v>
@@ -5582,7 +5582,7 @@
         <v>10</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y54" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5618,10 +5618,10 @@
         <v>11</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>11</v>
@@ -5648,7 +5648,7 @@
         <v>10</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U55" s="2" t="s">
         <v>10</v>
@@ -5696,7 +5696,7 @@
         <v>44</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>10</v>
@@ -5723,7 +5723,7 @@
         <v>11</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U56" s="2" t="s">
         <v>10</v>
@@ -5732,7 +5732,7 @@
         <v>11</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y56" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5771,7 +5771,7 @@
         <v>44</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>10</v>
@@ -5798,7 +5798,7 @@
         <v>10</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U57" s="2" t="s">
         <v>10</v>
@@ -5807,7 +5807,7 @@
         <v>11</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y57" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5843,10 +5843,10 @@
         <v>10</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>10</v>
@@ -5873,7 +5873,7 @@
         <v>11</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U58" s="2" t="s">
         <v>11</v>
@@ -5882,7 +5882,7 @@
         <v>10</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y58" s="3" t="str">
         <f t="shared" si="0"/>
@@ -5918,7 +5918,7 @@
         <v>10</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>14</v>
@@ -5948,7 +5948,7 @@
         <v>10</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U59" s="2" t="s">
         <v>10</v>
@@ -5996,7 +5996,7 @@
         <v>44</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>10</v>
@@ -6023,7 +6023,7 @@
         <v>10</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U60" s="2" t="s">
         <v>10</v>
@@ -6068,10 +6068,10 @@
         <v>10</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>11</v>
@@ -6098,7 +6098,7 @@
         <v>10</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U61" s="2" t="s">
         <v>10</v>
@@ -6107,7 +6107,7 @@
         <v>10</v>
       </c>
       <c r="W61" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y61" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6146,7 +6146,7 @@
         <v>59</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>11</v>
@@ -6173,7 +6173,7 @@
         <v>11</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U62" s="2" t="s">
         <v>10</v>
@@ -6218,10 +6218,10 @@
         <v>10</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>11</v>
@@ -6248,7 +6248,7 @@
         <v>10</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U63" s="2" t="s">
         <v>10</v>
@@ -6257,7 +6257,7 @@
         <v>10</v>
       </c>
       <c r="W63" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y63" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6293,10 +6293,10 @@
         <v>10</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>11</v>
@@ -6332,7 +6332,7 @@
         <v>10</v>
       </c>
       <c r="W64" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y64" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6371,7 +6371,7 @@
         <v>44</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>10</v>
@@ -6398,7 +6398,7 @@
         <v>11</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U65" s="2" t="s">
         <v>10</v>
@@ -6407,7 +6407,7 @@
         <v>11</v>
       </c>
       <c r="W65" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y65" s="3" t="str">
         <f t="shared" si="0"/>
@@ -6443,10 +6443,10 @@
         <v>11</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>10</v>
@@ -6473,7 +6473,7 @@
         <v>11</v>
       </c>
       <c r="T66" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U66" s="2" t="s">
         <v>11</v>
@@ -6518,10 +6518,10 @@
         <v>10</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>11</v>
@@ -6548,7 +6548,7 @@
         <v>10</v>
       </c>
       <c r="T67" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U67" s="2" t="s">
         <v>11</v>
@@ -6593,10 +6593,10 @@
         <v>10</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>10</v>
@@ -6623,7 +6623,7 @@
         <v>10</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U68" s="2" t="s">
         <v>10</v>
@@ -6632,7 +6632,7 @@
         <v>10</v>
       </c>
       <c r="W68" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y68" s="3" t="str">
         <f t="shared" ref="Y68:Y105" si="1">CONCATENATE("(",$A68,",",$B68,",",$C68,",",$D68,",",$E68,",",$F68,",",$G68,",",$H68,",",$I68,",",$J68,",",$K68,",",$L68,",",$M68,",",$N68,",",$O68,",",$P68,",",$Q68,",",$R68,",",$S68,",",$T68,",",$U68,",",$V68,",",$W68,"),")</f>
@@ -6668,10 +6668,10 @@
         <v>10</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>11</v>
@@ -6698,7 +6698,7 @@
         <v>10</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U69" s="2" t="s">
         <v>10</v>
@@ -6707,7 +6707,7 @@
         <v>11</v>
       </c>
       <c r="W69" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y69" s="3" t="str">
         <f t="shared" si="1"/>
@@ -6743,10 +6743,10 @@
         <v>10</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>10</v>
@@ -6773,7 +6773,7 @@
         <v>11</v>
       </c>
       <c r="T70" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U70" s="2" t="s">
         <v>10</v>
@@ -6818,10 +6818,10 @@
         <v>10</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>11</v>
@@ -6848,7 +6848,7 @@
         <v>10</v>
       </c>
       <c r="T71" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U71" s="2" t="s">
         <v>10</v>
@@ -6893,10 +6893,10 @@
         <v>10</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>11</v>
@@ -6943,8 +6943,8 @@
       <c r="A73" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>174</v>
+      <c r="B73" s="8" t="s">
+        <v>354</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>14</v>
@@ -6968,10 +6968,10 @@
         <v>10</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>10</v>
@@ -7011,19 +7011,19 @@
       </c>
       <c r="Y73" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>(70,'Cecile Terwilliger',null,null,null,true,true,true,false,'adult','scientist',false,'yellow','brown',false,false,false,false,false,'evil',false,false,null),</v>
+        <v>(70,Cecile Terwilliger',null,null,null,true,true,true,false,'adult','scientist',false,'yellow','brown',false,false,false,false,false,'evil',false,false,null),</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="D74" s="1" t="s">
         <v>14</v>
       </c>
@@ -7043,10 +7043,10 @@
         <v>10</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>11</v>
@@ -7091,10 +7091,10 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>14</v>
@@ -7121,7 +7121,7 @@
         <v>44</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>11</v>
@@ -7148,7 +7148,7 @@
         <v>10</v>
       </c>
       <c r="T75" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U75" s="2" t="s">
         <v>10</v>
@@ -7157,7 +7157,7 @@
         <v>11</v>
       </c>
       <c r="W75" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y75" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7166,14 +7166,14 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="D76" s="1" t="s">
         <v>14</v>
       </c>
@@ -7193,10 +7193,10 @@
         <v>10</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>11</v>
@@ -7241,11 +7241,11 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="C77" s="1" t="s">
         <v>14</v>
       </c>
@@ -7268,10 +7268,10 @@
         <v>10</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>11</v>
@@ -7298,7 +7298,7 @@
         <v>11</v>
       </c>
       <c r="T77" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U77" s="2" t="s">
         <v>10</v>
@@ -7307,7 +7307,7 @@
         <v>10</v>
       </c>
       <c r="W77" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y77" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7316,11 +7316,11 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
@@ -7343,10 +7343,10 @@
         <v>10</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>10</v>
@@ -7373,7 +7373,7 @@
         <v>10</v>
       </c>
       <c r="T78" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U78" s="2" t="s">
         <v>10</v>
@@ -7382,7 +7382,7 @@
         <v>11</v>
       </c>
       <c r="W78" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y78" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7391,11 +7391,11 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>14</v>
       </c>
@@ -7418,10 +7418,10 @@
         <v>10</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>11</v>
@@ -7448,7 +7448,7 @@
         <v>11</v>
       </c>
       <c r="T79" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U79" s="2" t="s">
         <v>10</v>
@@ -7457,7 +7457,7 @@
         <v>11</v>
       </c>
       <c r="W79" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y79" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7466,14 +7466,14 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
       </c>
@@ -7493,10 +7493,10 @@
         <v>10</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>11</v>
@@ -7541,11 +7541,11 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
@@ -7568,10 +7568,10 @@
         <v>10</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>11</v>
@@ -7598,7 +7598,7 @@
         <v>10</v>
       </c>
       <c r="T81" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U81" s="2" t="s">
         <v>10</v>
@@ -7616,11 +7616,11 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C82" s="1" t="s">
         <v>14</v>
       </c>
@@ -7643,10 +7643,10 @@
         <v>10</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>10</v>
@@ -7673,7 +7673,7 @@
         <v>10</v>
       </c>
       <c r="T82" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U82" s="2" t="s">
         <v>10</v>
@@ -7682,7 +7682,7 @@
         <v>10</v>
       </c>
       <c r="W82" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y82" s="3" t="str">
         <f t="shared" si="1"/>
@@ -7691,11 +7691,11 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C83" s="1" t="s">
         <v>14</v>
       </c>
@@ -7718,10 +7718,10 @@
         <v>10</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>10</v>
@@ -7748,7 +7748,7 @@
         <v>11</v>
       </c>
       <c r="T83" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U83" s="2" t="s">
         <v>10</v>
@@ -7766,10 +7766,10 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>14</v>
@@ -7796,7 +7796,7 @@
         <v>59</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>10</v>
@@ -7841,10 +7841,10 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>14</v>
@@ -7898,7 +7898,7 @@
         <v>10</v>
       </c>
       <c r="T85" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U85" s="2" t="s">
         <v>10</v>
@@ -7916,10 +7916,10 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>14</v>
@@ -7973,7 +7973,7 @@
         <v>10</v>
       </c>
       <c r="T86" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U86" s="2" t="s">
         <v>10</v>
@@ -7991,10 +7991,10 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>14</v>
@@ -8048,7 +8048,7 @@
         <v>10</v>
       </c>
       <c r="T87" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U87" s="2" t="s">
         <v>10</v>
@@ -8066,10 +8066,10 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>14</v>
@@ -8123,7 +8123,7 @@
         <v>10</v>
       </c>
       <c r="T88" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U88" s="2" t="s">
         <v>10</v>
@@ -8141,10 +8141,10 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>14</v>
@@ -8171,7 +8171,7 @@
         <v>59</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>10</v>
@@ -8198,7 +8198,7 @@
         <v>10</v>
       </c>
       <c r="T89" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U89" s="2" t="s">
         <v>10</v>
@@ -8216,10 +8216,10 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>14</v>
@@ -8291,10 +8291,10 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>14</v>
@@ -8321,7 +8321,7 @@
         <v>59</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>10</v>
@@ -8348,7 +8348,7 @@
         <v>10</v>
       </c>
       <c r="T91" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U91" s="2" t="s">
         <v>11</v>
@@ -8366,10 +8366,10 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>14</v>
@@ -8396,7 +8396,7 @@
         <v>59</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>10</v>
@@ -8423,7 +8423,7 @@
         <v>10</v>
       </c>
       <c r="T92" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U92" s="2" t="s">
         <v>10</v>
@@ -8441,10 +8441,10 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>14</v>
@@ -8471,7 +8471,7 @@
         <v>59</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>10</v>
@@ -8516,10 +8516,10 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>14</v>
@@ -8546,7 +8546,7 @@
         <v>59</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>10</v>
@@ -8582,7 +8582,7 @@
         <v>10</v>
       </c>
       <c r="W94" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y94" s="3" t="str">
         <f t="shared" si="1"/>
@@ -8591,10 +8591,10 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>14</v>
@@ -8621,7 +8621,7 @@
         <v>59</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>10</v>
@@ -8666,10 +8666,10 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>14</v>
@@ -8696,7 +8696,7 @@
         <v>59</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>10</v>
@@ -8723,7 +8723,7 @@
         <v>10</v>
       </c>
       <c r="T96" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U96" s="2" t="s">
         <v>10</v>
@@ -8741,10 +8741,10 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>14</v>
@@ -8771,7 +8771,7 @@
         <v>59</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>10</v>
@@ -8798,7 +8798,7 @@
         <v>10</v>
       </c>
       <c r="T97" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U97" s="2" t="s">
         <v>10</v>
@@ -8816,10 +8816,10 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>14</v>
@@ -8846,7 +8846,7 @@
         <v>59</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>10</v>
@@ -8873,7 +8873,7 @@
         <v>10</v>
       </c>
       <c r="T98" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U98" s="2" t="s">
         <v>10</v>
@@ -8891,13 +8891,13 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>14</v>
@@ -8921,7 +8921,7 @@
         <v>59</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>10</v>
@@ -8966,10 +8966,10 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>14</v>
@@ -8996,7 +8996,7 @@
         <v>59</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>10</v>
@@ -9023,7 +9023,7 @@
         <v>10</v>
       </c>
       <c r="T100" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U100" s="2" t="s">
         <v>10</v>
@@ -9032,7 +9032,7 @@
         <v>10</v>
       </c>
       <c r="W100" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y100" s="3" t="str">
         <f t="shared" si="1"/>
@@ -9041,10 +9041,10 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>14</v>
@@ -9071,7 +9071,7 @@
         <v>44</v>
       </c>
       <c r="K101" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>11</v>
@@ -9116,14 +9116,14 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="D102" s="1" t="s">
         <v>14</v>
       </c>
@@ -9143,10 +9143,10 @@
         <v>10</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K102" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>11</v>
@@ -9173,7 +9173,7 @@
         <v>10</v>
       </c>
       <c r="T102" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U102" s="2" t="s">
         <v>10</v>
@@ -9182,7 +9182,7 @@
         <v>10</v>
       </c>
       <c r="W102" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y102" s="3" t="str">
         <f t="shared" si="1"/>
@@ -9191,10 +9191,10 @@
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>14</v>
@@ -9221,7 +9221,7 @@
         <v>44</v>
       </c>
       <c r="K103" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>11</v>
@@ -9248,7 +9248,7 @@
         <v>10</v>
       </c>
       <c r="T103" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U103" s="2" t="s">
         <v>10</v>
@@ -9266,11 +9266,11 @@
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="C104" s="1" t="s">
         <v>14</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>11</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>14</v>
@@ -9323,7 +9323,7 @@
         <v>10</v>
       </c>
       <c r="T104" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>10</v>
@@ -9341,11 +9341,11 @@
     </row>
     <row r="105" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="C105" s="1" t="s">
         <v>14</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>10</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>14</v>
@@ -9453,21 +9453,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9559,21 +9559,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9701,18 +9701,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9741,18 +9741,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9781,18 +9781,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9821,18 +9821,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9861,18 +9861,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9901,18 +9901,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9941,18 +9941,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -9981,18 +9981,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10021,18 +10021,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10061,18 +10061,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10101,18 +10101,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10141,18 +10141,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10181,18 +10181,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -10227,21 +10227,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E2" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -10249,10 +10249,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E3" s="3" t="str">
         <f>CONCATENATE("(",$A3,",",$B3,",",$C3,"),")</f>
@@ -10261,13 +10261,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" ref="E4:E5" si="0">CONCATENATE("(",$A4,",",$B4,",",$C4,"),")</f>
@@ -10279,10 +10279,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -10322,27 +10322,27 @@
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -10354,7 +10354,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -10366,7 +10366,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -10378,7 +10378,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -10390,7 +10390,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -10402,7 +10402,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -10414,7 +10414,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -10426,7 +10426,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -10438,7 +10438,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -10450,7 +10450,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -10462,7 +10462,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -10474,7 +10474,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -10486,7 +10486,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -10498,7 +10498,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -10510,7 +10510,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -10522,7 +10522,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -10534,7 +10534,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -10546,7 +10546,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -10558,7 +10558,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -10570,7 +10570,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -10582,7 +10582,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -10594,7 +10594,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -10606,7 +10606,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -10618,7 +10618,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -10630,7 +10630,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -10681,18 +10681,18 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>